<commit_message>
Se cambio de infobae a facebook
</commit_message>
<xml_diff>
--- a/IntegracionDemo1/Default.xlsx
+++ b/IntegracionDemo1/Default.xlsx
@@ -469,14 +469,16 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>